<commit_message>
update@pc@7.58-30092016 moved experimental results to a separate folder
</commit_message>
<xml_diff>
--- a/RStudioProjects/mbDiscoveryR/test results.xlsx
+++ b/RStudioProjects/mbDiscoveryR/test results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="synthetic" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,12 @@
     <sheet name="7.2.3.1" sheetId="14" r:id="rId10"/>
     <sheet name="34.4.4.1" sheetId="15" r:id="rId11"/>
     <sheet name="50.5.6.1" sheetId="5" r:id="rId12"/>
-    <sheet name="100.5.6.1" sheetId="10" r:id="rId13"/>
+    <sheet name="70.6.5.1" sheetId="10" r:id="rId13"/>
+    <sheet name="90.5.6.1" sheetId="19" r:id="rId14"/>
+    <sheet name="150.5.6.1" sheetId="20" r:id="rId15"/>
+    <sheet name="optimize alpha" sheetId="18" r:id="rId16"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId17"/>
+    <sheet name="Sheet5" sheetId="21" r:id="rId18"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="1035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2336" uniqueCount="1231">
   <si>
     <t>BN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3975,14 +3980,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>iamb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pcmb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mml</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4053,13 +4050,701 @@
   <si>
     <t>0.84 $\pm$ 0</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.46 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.11 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.11 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.15 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.43 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.13 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.13 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.09 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.17 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.45 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.12 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.14 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.14 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.51 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.12 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.08 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.16 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.07 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.18 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.65 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.27 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.27 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.87 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.87 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.32 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.32 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.32 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.84 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.36 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.36 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.72 $\pm$ 0.03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.21 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.91 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.91 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.28 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.73 $\pm$ 0.03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.26 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.85 $\pm$ 0.03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.33 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.72 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.96 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.97 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.06 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.96 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>precision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>recall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>distance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f-measure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.98 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.05 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alarm 10000 pcmb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alarm 1000 pcmb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.91 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.78 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.27 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.82 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.92 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.87 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.19 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.90 0.02</t>
+  </si>
+  <si>
+    <t>3  0.20 0.02</t>
+  </si>
+  <si>
+    <t>4  0.87 0.01</t>
+  </si>
+  <si>
+    <t>0.88 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.20 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2  0.89 0.01</t>
+  </si>
+  <si>
+    <t>1  0.89 0.02</t>
+  </si>
+  <si>
+    <t>0.71 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.34 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.79 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.39 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.41 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.74 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.74 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.78 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.83 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.34 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.34 $\pm$ 0.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8 $\pm$ 0.03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.26 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.26 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.82 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.82 $\pm$ 0.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.75 $\pm$ 0.03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70-5-6-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1  0.87 0.02</t>
+  </si>
+  <si>
+    <t>3  0.21 0.02</t>
+  </si>
+  <si>
+    <t>4  0.86 0.01</t>
+  </si>
+  <si>
+    <t>90-5-6-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>150-5-6-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.16 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.29 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>1.17 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.3 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.39 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>1.13 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.33 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>1.15 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.24 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.43 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.96 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.28 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.67 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.23 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.57 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.31 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.87 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.49 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.37 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.86 $\pm$ 0.01</t>
+  </si>
+  <si>
+    <t>0.75 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.81 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.35 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t>0.77 $\pm$ 0.03</t>
+  </si>
+  <si>
+    <t>0.4 $\pm$ 0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alarm 500 mml </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alarm 500 pcmb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1  0.89 0.01</t>
+  </si>
+  <si>
+    <t>2  0.71 0.02</t>
+  </si>
+  <si>
+    <t>alarm 500 iamb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3  0.37 0.02</t>
+  </si>
+  <si>
+    <t>4  0.75 0.01</t>
+  </si>
+  <si>
+    <t>2  0.65 0.01</t>
+  </si>
+  <si>
+    <t>4  0.72 0.01</t>
+  </si>
+  <si>
+    <t>2  0.81 0.02</t>
+  </si>
+  <si>
+    <t>1  0.88 0.01</t>
+  </si>
+  <si>
+    <t>small</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>medium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>large</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>very large</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7-3-2-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>34-4-4-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50-5-6-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insurance, Alarm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hailfinder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70-5-6-1, 90-5-6-1, 150-5-6-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100, 500, 1000, 10000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100, 500, 1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Real models
+(real parameters)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Artificial models
+(uniform prior)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Real models
+(uniform prior)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1  0.90 0.01</t>
+  </si>
+  <si>
+    <t>2  0.66 0.01</t>
+  </si>
+  <si>
+    <t>3  0.39 0.02</t>
+  </si>
+  <si>
+    <t>4  0.73 0.01</t>
+  </si>
+  <si>
+    <t>2  0.64 0.01</t>
+  </si>
+  <si>
+    <t>3  0.41 0.02</t>
+  </si>
+  <si>
+    <t>4  0.70 0.01</t>
+  </si>
+  <si>
+    <t>2  0.61 0.01</t>
+  </si>
+  <si>
+    <t>3  0.44 0.02</t>
+  </si>
+  <si>
+    <t>4  0.68 0.01</t>
+  </si>
+  <si>
+    <t>3  0.38 0.02</t>
+  </si>
+  <si>
+    <t>1  0.86 0.01</t>
+  </si>
+  <si>
+    <t>2  0.67 0.02</t>
+  </si>
+  <si>
+    <t>3  0.40 0.02</t>
+  </si>
+  <si>
+    <t>4  0.72 0.02</t>
+  </si>
+  <si>
+    <t>1  0.85 0.01</t>
+  </si>
+  <si>
+    <t>1  0.84 0.01</t>
+  </si>
+  <si>
+    <t>2  0.72 0.02</t>
+  </si>
+  <si>
+    <t>4  0.75 0.02</t>
+  </si>
+  <si>
+    <t>1  0.82 0.01</t>
+  </si>
+  <si>
+    <t>2  0.74 0.02</t>
+  </si>
+  <si>
+    <t>4  0.74 0.02</t>
+  </si>
+  <si>
+    <t>4  0.74 0.01</t>
+  </si>
+  <si>
+    <t>1  0.79 0.02</t>
+  </si>
+  <si>
+    <t>2  0.75 0.02</t>
+  </si>
+  <si>
+    <t>2  0.68 0.02</t>
+  </si>
+  <si>
+    <t>2  0.69 0.02</t>
+  </si>
+  <si>
+    <t>3  0.36 0.02</t>
+  </si>
+  <si>
+    <t>2  0.70 0.02</t>
+  </si>
+  <si>
+    <t>1  0.59 0.01</t>
+  </si>
+  <si>
+    <t>2  0.78 0.01</t>
+  </si>
+  <si>
+    <t>3  0.54 0.01</t>
+  </si>
+  <si>
+    <t>4  0.62 0.01</t>
+  </si>
+  <si>
+    <t>1  0.75 0.01</t>
+  </si>
+  <si>
+    <t>3  0.42 0.02</t>
+  </si>
+  <si>
+    <t>4  0.71 0.01</t>
+  </si>
+  <si>
+    <t>2  0.73 0.02</t>
+  </si>
+  <si>
+    <t>1  0.79 0.01</t>
+  </si>
+  <si>
+    <t>1  0.83 0.01</t>
+  </si>
+  <si>
+    <t>2  0.58 0.02</t>
+  </si>
+  <si>
+    <t>3  0.49 0.02</t>
+  </si>
+  <si>
+    <t>4  0.65 0.02</t>
+  </si>
+  <si>
+    <t>2  0.63 0.02</t>
+  </si>
+  <si>
+    <t>4  0.69 0.02</t>
+  </si>
+  <si>
+    <t>2  0.65 0.02</t>
+  </si>
+  <si>
+    <t>4  0.71 0.02</t>
+  </si>
+  <si>
+    <t>2  0.66 0.02</t>
+  </si>
+  <si>
+    <t>1  0.74 0.01</t>
+  </si>
+  <si>
+    <t>2  0.77 0.02</t>
+  </si>
+  <si>
+    <t>1  0.68 0.02</t>
+  </si>
+  <si>
+    <t>2  0.79 0.02</t>
+  </si>
+  <si>
+    <t>1  0.57 0.02</t>
+  </si>
+  <si>
+    <t>3  0.52 0.02</t>
+  </si>
+  <si>
+    <t>4  0.63 0.02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4127,8 +4812,36 @@
       <name val="宋体"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4153,8 +4866,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -4162,8 +4885,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4263,8 +5019,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4325,8 +5087,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="34" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="33" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="33" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="35">
+    <cellStyle name="好" xfId="33" builtinId="26"/>
     <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -4344,6 +5149,7 @@
     <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="注释" xfId="34" builtinId="10"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -4762,11 +5568,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223806224"/>
-        <c:axId val="223806784"/>
+        <c:axId val="227392928"/>
+        <c:axId val="227393488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="223806224"/>
+        <c:axId val="227392928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4809,7 +5615,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223806784"/>
+        <c:crossAx val="227393488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4817,7 +5623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="223806784"/>
+        <c:axId val="227393488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4868,7 +5674,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223806224"/>
+        <c:crossAx val="227392928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5336,11 +6142,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223811264"/>
-        <c:axId val="223811824"/>
+        <c:axId val="228013056"/>
+        <c:axId val="228013616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="223811264"/>
+        <c:axId val="228013056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5383,7 +6189,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223811824"/>
+        <c:crossAx val="228013616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5391,7 +6197,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="223811824"/>
+        <c:axId val="228013616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5442,7 +6248,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223811264"/>
+        <c:crossAx val="228013056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5730,11 +6536,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="224128736"/>
-        <c:axId val="224129296"/>
+        <c:axId val="228016976"/>
+        <c:axId val="228017536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="224128736"/>
+        <c:axId val="228016976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5776,7 +6582,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224129296"/>
+        <c:crossAx val="228017536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5784,7 +6590,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224129296"/>
+        <c:axId val="228017536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5835,7 +6641,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224128736"/>
+        <c:crossAx val="228016976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6123,11 +6929,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="224132096"/>
-        <c:axId val="224132656"/>
+        <c:axId val="228089216"/>
+        <c:axId val="228089776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="224132096"/>
+        <c:axId val="228089216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6169,7 +6975,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224132656"/>
+        <c:crossAx val="228089776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6177,7 +6983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224132656"/>
+        <c:axId val="228089776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6228,7 +7034,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224132096"/>
+        <c:crossAx val="228089216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6349,6 +7155,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6389,11 +7196,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100.5.6.1'!$B$1</c:f>
+              <c:f>'70.6.5.1'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>iamb</c:v>
+                  <c:v>Instances</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6424,21 +7231,12 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'100.5.6.1'!$B$2:$B$5</c:f>
+              <c:f>'70.6.5.1'!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.47</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6450,11 +7248,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100.5.6.1'!$C$1</c:f>
+              <c:f>'70.6.5.1'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>pcmb</c:v>
+                  <c:v>Algorithm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6485,21 +7283,12 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'100.5.6.1'!$C$2:$C$5</c:f>
+              <c:f>'70.6.5.1'!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.77</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.61</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.27</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.15</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6511,11 +7300,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100.5.6.1'!$D$1</c:f>
+              <c:f>'70.6.5.1'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mml</c:v>
+                  <c:v>Precision</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6546,21 +7335,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'100.5.6.1'!$D$2:$D$5</c:f>
+              <c:f>'70.6.5.1'!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.48</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6577,11 +7366,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="224913744"/>
-        <c:axId val="224914304"/>
+        <c:axId val="228093136"/>
+        <c:axId val="228093696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="224913744"/>
+        <c:axId val="228093136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6623,7 +7412,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224914304"/>
+        <c:crossAx val="228093696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6631,7 +7420,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224914304"/>
+        <c:axId val="228093696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6682,7 +7471,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224913744"/>
+        <c:crossAx val="228093136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6696,6 +7485,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6803,6 +7593,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6843,11 +7634,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100.5.6.1'!$B$6</c:f>
+              <c:f>'70.6.5.1'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>iamb</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6878,22 +7669,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'100.5.6.1'!$B$7:$B$10</c:f>
+              <c:f>'70.6.5.1'!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.48</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.35</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6904,11 +7683,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100.5.6.1'!$C$6</c:f>
+              <c:f>'70.6.5.1'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>pcmb</c:v>
+                  <c:v>IAMB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6939,21 +7718,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'100.5.6.1'!$C$7:$C$10</c:f>
+              <c:f>'70.6.5.1'!$C$3:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.92</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.46</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6965,11 +7744,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100.5.6.1'!$D$6</c:f>
+              <c:f>'70.6.5.1'!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mml</c:v>
+                  <c:v>0.51 $\pm$ 0.02</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7000,21 +7779,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'100.5.6.1'!$D$7:$D$10</c:f>
+              <c:f>'70.6.5.1'!$D$7:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.83</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7031,11 +7810,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="224918224"/>
-        <c:axId val="224918784"/>
+        <c:axId val="229527536"/>
+        <c:axId val="229528096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="224918224"/>
+        <c:axId val="229527536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7077,7 +7856,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224918784"/>
+        <c:crossAx val="229528096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7085,7 +7864,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224918784"/>
+        <c:axId val="229528096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7136,7 +7915,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224918224"/>
+        <c:crossAx val="229527536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7150,6 +7929,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7257,6 +8037,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7297,12 +8078,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100.5.6.1'!$B$11</c:f>
+              <c:f>'70.6.5.1'!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>iamb</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -7332,24 +8110,12 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'100.5.6.1'!$B$12:$B$16</c:f>
+              <c:f>'70.6.5.1'!$B$8:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.04</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.67</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.44</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.41</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7361,11 +8127,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100.5.6.1'!$C$11</c:f>
+              <c:f>'70.6.5.1'!$C$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>pcmb</c:v>
+                  <c:v>MMLCPT (sym)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7396,24 +8162,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'100.5.6.1'!$C$12:$C$16</c:f>
+              <c:f>'70.6.5.1'!$C$8:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.06</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.81</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7425,11 +8191,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100.5.6.1'!$D$11</c:f>
+              <c:f>'70.6.5.1'!$D$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mml</c:v>
+                  <c:v>0.72 $\pm$ 0.02</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7460,24 +8226,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'100.5.6.1'!$D$12:$D$16</c:f>
+              <c:f>'70.6.5.1'!$D$12:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7494,11 +8260,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="225466496"/>
-        <c:axId val="225467056"/>
+        <c:axId val="229532016"/>
+        <c:axId val="229532576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="225466496"/>
+        <c:axId val="229532016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7540,7 +8306,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225467056"/>
+        <c:crossAx val="229532576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7548,7 +8314,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="225467056"/>
+        <c:axId val="229532576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7599,7 +8365,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225466496"/>
+        <c:crossAx val="229532016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7613,6 +8379,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11628,7 +12395,9 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -11658,7 +12427,9 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="图表 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -11688,7 +12459,9 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="图表 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -13779,7 +14552,7 @@
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:G35"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
@@ -14544,10 +15317,2218 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B2" s="4">
+        <v>100</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>1036</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>861</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>1041</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>1044</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>1044</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>1049</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>1051</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23">
+        <v>500</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>1057</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>1062</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>1103</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>1108</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>1115</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>1117</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>1118</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23">
+        <v>10000</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D21" s="26"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26">
+        <v>20000</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="C27" t="s">
+        <v>283</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="C29" t="s">
+        <v>284</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="4:7">
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+    </row>
+    <row r="34" spans="4:7">
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+    </row>
+    <row r="35" spans="4:7">
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="17.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="4" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B2" s="4">
+        <v>100</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>1036</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>861</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>1041</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>1044</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>1044</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>1049</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>1051</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23">
+        <v>500</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>1057</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>1062</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>1103</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>1108</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>1115</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>1117</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>1118</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23">
+        <v>10000</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D21" s="26"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26">
+        <v>20000</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="C27" t="s">
+        <v>283</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="C29" t="s">
+        <v>284</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="17.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B2" s="4">
+        <v>100</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>1125</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>861</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>1125</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>1125</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>1130</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23">
+        <v>500</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>852</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>884</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>1135</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>851</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>881</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>851</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>881</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>1067</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>1114</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>1141</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>1144</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>1146</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>1146</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>869</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>1060</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B1">
+        <v>0.01</v>
+      </c>
+      <c r="C1">
+        <v>0.03</v>
+      </c>
+      <c r="D1">
+        <v>0.05</v>
+      </c>
+      <c r="E1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F1">
+        <v>0.09</v>
+      </c>
+      <c r="G1">
+        <v>0.11</v>
+      </c>
+      <c r="H1">
+        <v>0.13</v>
+      </c>
+      <c r="I1">
+        <v>0.15</v>
+      </c>
+      <c r="J1">
+        <v>0.17</v>
+      </c>
+      <c r="K1">
+        <v>0.19</v>
+      </c>
+      <c r="L1">
+        <v>0.21</v>
+      </c>
+      <c r="M1">
+        <v>0.23</v>
+      </c>
+      <c r="N1">
+        <v>0.25</v>
+      </c>
+      <c r="O1">
+        <v>0.27</v>
+      </c>
+      <c r="P1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B8">
+        <v>0.01</v>
+      </c>
+      <c r="C8" s="29">
+        <v>0.03</v>
+      </c>
+      <c r="D8">
+        <v>0.05</v>
+      </c>
+      <c r="E8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.09</v>
+      </c>
+      <c r="G8">
+        <v>0.11</v>
+      </c>
+      <c r="H8">
+        <v>0.13</v>
+      </c>
+      <c r="I8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1101</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1120</v>
+      </c>
+      <c r="G9" s="28"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1100</v>
+      </c>
+      <c r="G10" s="28"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1096</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G11" s="28"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G12" s="28"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B15" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="C15" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>1177</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>1152</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>1178</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>1181</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>1182</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>1185</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="7"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>1183</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B21">
+        <v>1E-3</v>
+      </c>
+      <c r="C21">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D21">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E21">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="G21" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="H21">
+        <v>0.05</v>
+      </c>
+      <c r="I21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J21">
+        <v>0.09</v>
+      </c>
+      <c r="K21">
+        <v>0.15</v>
+      </c>
+      <c r="L21">
+        <v>0.2</v>
+      </c>
+      <c r="M21">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>1188</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>1192</v>
+      </c>
+      <c r="H22" t="s">
+        <v>1193</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1196</v>
+      </c>
+      <c r="J22" t="s">
+        <v>1200</v>
+      </c>
+      <c r="K22" t="s">
+        <v>1224</v>
+      </c>
+      <c r="L22" t="s">
+        <v>1226</v>
+      </c>
+      <c r="M22" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1221</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>1189</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>1153</v>
+      </c>
+      <c r="H23" t="s">
+        <v>1194</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1197</v>
+      </c>
+      <c r="J23" t="s">
+        <v>1201</v>
+      </c>
+      <c r="K23" t="s">
+        <v>1225</v>
+      </c>
+      <c r="L23" t="s">
+        <v>1227</v>
+      </c>
+      <c r="M23" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>1155</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1155</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1155</v>
+      </c>
+      <c r="J24" t="s">
+        <v>1187</v>
+      </c>
+      <c r="K24" t="s">
+        <v>1182</v>
+      </c>
+      <c r="L24" t="s">
+        <v>1185</v>
+      </c>
+      <c r="M24" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1222</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1191</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>1191</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>1156</v>
+      </c>
+      <c r="H25" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I25" t="s">
+        <v>1198</v>
+      </c>
+      <c r="J25" t="s">
+        <v>1198</v>
+      </c>
+      <c r="K25" t="s">
+        <v>1158</v>
+      </c>
+      <c r="L25" t="s">
+        <v>1220</v>
+      </c>
+      <c r="M25" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="B26" s="2"/>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B27" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C27" s="7">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="D27">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E27" s="29">
+        <v>1E-3</v>
+      </c>
+      <c r="F27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G27">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H27">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I27">
+        <v>0.01</v>
+      </c>
+      <c r="J27">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1192</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1196</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1214</v>
+      </c>
+      <c r="I28" t="s">
+        <v>1210</v>
+      </c>
+      <c r="J28" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>1205</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1213</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1197</v>
+      </c>
+      <c r="H29" t="s">
+        <v>1201</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1201</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1187</v>
+      </c>
+      <c r="H30" t="s">
+        <v>1190</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1211</v>
+      </c>
+      <c r="J30" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1156</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1199</v>
+      </c>
+      <c r="H31" t="s">
+        <v>1180</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1212</v>
+      </c>
+      <c r="J31" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
@@ -14560,13 +17541,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>1015</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1016</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -14627,13 +17608,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>1015</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1016</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -14697,13 +17678,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
         <v>1015</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1016</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -14812,13 +17793,456 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="5" max="8" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C1">
+        <v>0.01</v>
+      </c>
+      <c r="E1" t="str">
+        <f>CONCATENATE(B1, " $\pm$ ", C1)</f>
+        <v>0.57 $\pm$ 0.01</v>
+      </c>
+      <c r="F1" t="str">
+        <f>CONCATENATE(B2, " $\pm$ ", C2)</f>
+        <v>0.31 $\pm$ 0.01</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE(B3, " $\pm$ ", C3)</f>
+        <v>0.87 $\pm$ 0.01</v>
+      </c>
+      <c r="H1" t="str">
+        <f>CONCATENATE(B4, " $\pm$ ", C4)</f>
+        <v>0.33 $\pm$ 0.01</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0.31</v>
+      </c>
+      <c r="C2">
+        <v>0.01</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE(B5, " $\pm$ ", C5)</f>
+        <v>0.49 $\pm$ 0.01</v>
+      </c>
+      <c r="F2" t="str">
+        <f>CONCATENATE(B6, " $\pm$ ", C6)</f>
+        <v>0.37 $\pm$ 0.02</v>
+      </c>
+      <c r="G2" t="str">
+        <f>CONCATENATE(B7, " $\pm$ ", C7)</f>
+        <v>0.86 $\pm$ 0.01</v>
+      </c>
+      <c r="H2" t="str">
+        <f>CONCATENATE(B8, " $\pm$ ", C8)</f>
+        <v>0.36 $\pm$ 0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="27">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0.87</v>
+      </c>
+      <c r="C3">
+        <v>0.01</v>
+      </c>
+      <c r="E3" t="str">
+        <f>CONCATENATE(B9, " $\pm$ ", C9)</f>
+        <v>0.75 $\pm$ 0.02</v>
+      </c>
+      <c r="F3" t="str">
+        <f>CONCATENATE(B10, " $\pm$ ", C10)</f>
+        <v>0.3 $\pm$ 0.01</v>
+      </c>
+      <c r="G3" t="str">
+        <f>CONCATENATE(B11, " $\pm$ ", C11)</f>
+        <v>0.81 $\pm$ 0.02</v>
+      </c>
+      <c r="H3" t="str">
+        <f>CONCATENATE(B12, " $\pm$ ", C12)</f>
+        <v>0.37 $\pm$ 0.02</v>
+      </c>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32" t="s">
+        <v>1175</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>1174</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>1176</v>
+      </c>
+      <c r="N3" s="33" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.33</v>
+      </c>
+      <c r="C4">
+        <v>0.01</v>
+      </c>
+      <c r="E4" t="str">
+        <f>CONCATENATE(B13, " $\pm$ ", C13)</f>
+        <v>0.75 $\pm$ 0.02</v>
+      </c>
+      <c r="F4" t="str">
+        <f>CONCATENATE(B14, " $\pm$ ", C14)</f>
+        <v>0.3 $\pm$ 0.01</v>
+      </c>
+      <c r="G4" t="str">
+        <f>CONCATENATE(B15, " $\pm$ ", C15)</f>
+        <v>0.81 $\pm$ 0.02</v>
+      </c>
+      <c r="H4" t="str">
+        <f>CONCATENATE(B16, " $\pm$ ", C16)</f>
+        <v>0.37 $\pm$ 0.02</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>1161</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>1165</v>
+      </c>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.49</v>
+      </c>
+      <c r="C5">
+        <v>0.01</v>
+      </c>
+      <c r="E5" t="str">
+        <f>CONCATENATE(B17, " $\pm$ ", C17)</f>
+        <v>0.74 $\pm$ 0.02</v>
+      </c>
+      <c r="F5" t="str">
+        <f>CONCATENATE(B18, " $\pm$ ", C18)</f>
+        <v>0.28 $\pm$ 0.01</v>
+      </c>
+      <c r="G5" t="str">
+        <f>CONCATENATE(B19, " $\pm$ ", C19)</f>
+        <v>0.82 $\pm$ 0.02</v>
+      </c>
+      <c r="H5" t="str">
+        <f>CONCATENATE(B20, " $\pm$ ", C20)</f>
+        <v>0.35 $\pm$ 0.02</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>1162</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>1166</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>1168</v>
+      </c>
+      <c r="M5" s="31" t="s">
+        <v>1168</v>
+      </c>
+      <c r="N5" s="31" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>0.37</v>
+      </c>
+      <c r="C6">
+        <v>0.02</v>
+      </c>
+      <c r="E6" t="str">
+        <f>CONCATENATE(B21, " $\pm$ ", C21)</f>
+        <v>0.76 $\pm$ 0.02</v>
+      </c>
+      <c r="F6" t="str">
+        <f>CONCATENATE(B22, " $\pm$ ", C22)</f>
+        <v>0.32 $\pm$ 0.02</v>
+      </c>
+      <c r="G6" t="str">
+        <f>CONCATENATE(B23, " $\pm$ ", C23)</f>
+        <v>0.77 $\pm$ 0.03</v>
+      </c>
+      <c r="H6" t="str">
+        <f>CONCATENATE(B24, " $\pm$ ", C24)</f>
+        <v>0.4 $\pm$ 0.02</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>1163</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>1167</v>
+      </c>
+      <c r="L6" s="31" t="s">
+        <v>1169</v>
+      </c>
+      <c r="M6" s="31" t="s">
+        <v>1169</v>
+      </c>
+      <c r="N6" s="31" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0.86</v>
+      </c>
+      <c r="C7">
+        <v>0.01</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>1164</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>1170</v>
+      </c>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>0.36</v>
+      </c>
+      <c r="C8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0.75</v>
+      </c>
+      <c r="C9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0.3</v>
+      </c>
+      <c r="C10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>0.81</v>
+      </c>
+      <c r="C11">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>0.37</v>
+      </c>
+      <c r="C12">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0.75</v>
+      </c>
+      <c r="C13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0.3</v>
+      </c>
+      <c r="C14">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>0.81</v>
+      </c>
+      <c r="C15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>0.37</v>
+      </c>
+      <c r="C16">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>0.74</v>
+      </c>
+      <c r="C17">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C18">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>0.82</v>
+      </c>
+      <c r="C19">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>0.35</v>
+      </c>
+      <c r="C20">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>0.76</v>
+      </c>
+      <c r="C21">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>0.32</v>
+      </c>
+      <c r="C22">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>0.77</v>
+      </c>
+      <c r="C23">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>0.4</v>
+      </c>
+      <c r="C24">
+        <v>0.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -20776,8 +24200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -21170,13 +24594,13 @@
         <v>25</v>
       </c>
       <c r="D20" s="10" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>1017</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>1018</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>1019</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>1020</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>1002</v>
@@ -21189,13 +24613,13 @@
         <v>283</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>1014</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>1004</v>
@@ -21208,16 +24632,16 @@
         <v>26</v>
       </c>
       <c r="D22" s="6" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>1023</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="G22" s="6" t="s">
         <v>1024</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -21227,16 +24651,16 @@
         <v>284</v>
       </c>
       <c r="D23" s="6" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>1023</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="G23" s="6" t="s">
         <v>1024</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -21246,16 +24670,16 @@
         <v>27</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>1027</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="G24" s="6" t="s">
         <v>1028</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>1029</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>1030</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -21265,16 +24689,16 @@
         <v>28</v>
       </c>
       <c r="D25" s="6" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>1031</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="G25" s="6" t="s">
         <v>1032</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>1033</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>1034</v>
       </c>
     </row>
     <row r="26" spans="1:7">

</xml_diff>